<commit_message>
improves data_to_dict and update data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clementboloch/Documents/OpenClassrooms/Projet 7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7610074B-1B75-A444-AE8F-BD2AF5DD51A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7CC668-28E3-644F-8C39-8A4435727994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{063A6BE7-A2EC-6A4E-997C-B671AB71AA1B}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Coût par action (en euros)</t>
   </si>
   <si>
-    <t>Bénéfice (après 2 ans)</t>
-  </si>
-  <si>
     <t>Action-1</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Action-20</t>
+  </si>
+  <si>
+    <t>Bénéfice (après 2 ans)</t>
   </si>
 </sst>
 </file>
@@ -473,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3026227E-9DC0-1541-8D45-4F0E5B43E2FB}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -486,7 +486,7 @@
     <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21">
+    <row r="1" spans="1:8" ht="21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,12 +494,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="20">
+      <c r="A2" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>20</v>
@@ -508,9 +508,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20">
+    <row r="3" spans="1:8" ht="20">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>30</v>
@@ -519,9 +519,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20">
+    <row r="4" spans="1:8" ht="20">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>50</v>
@@ -530,9 +530,9 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20">
+    <row r="5" spans="1:8" ht="20">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>70</v>
@@ -541,9 +541,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20">
+    <row r="6" spans="1:8" ht="21">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>60</v>
@@ -551,10 +551,11 @@
       <c r="C6" s="3">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="20">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="20">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>80</v>
@@ -563,9 +564,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20">
+    <row r="8" spans="1:8" ht="20">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>22</v>
@@ -574,9 +575,9 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20">
+    <row r="9" spans="1:8" ht="20">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>26</v>
@@ -585,9 +586,9 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20">
+    <row r="10" spans="1:8" ht="20">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>48</v>
@@ -596,9 +597,9 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20">
+    <row r="11" spans="1:8" ht="20">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2">
         <v>34</v>
@@ -607,9 +608,9 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20">
+    <row r="12" spans="1:8" ht="20">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2">
         <v>42</v>
@@ -618,20 +619,20 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20">
+    <row r="13" spans="1:8" ht="20">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
         <v>110</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="20">
+      <c r="A14" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="20">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="B14" s="2">
         <v>38</v>
@@ -640,9 +641,9 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20">
+    <row r="15" spans="1:8" ht="20">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -651,9 +652,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20">
+    <row r="16" spans="1:8" ht="20">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <v>18</v>
@@ -664,7 +665,7 @@
     </row>
     <row r="17" spans="1:3" ht="20">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>8</v>
@@ -675,7 +676,7 @@
     </row>
     <row r="18" spans="1:3" ht="20">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <v>4</v>
@@ -686,7 +687,7 @@
     </row>
     <row r="19" spans="1:3" ht="20">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2">
         <v>10</v>
@@ -697,10 +698,10 @@
     </row>
     <row r="20" spans="1:3" ht="20">
       <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C20" s="3">
         <v>0.21</v>
@@ -708,7 +709,7 @@
     </row>
     <row r="21" spans="1:3" ht="20">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2">
         <v>114</v>

</xml_diff>